<commit_message>
Update Matriz de Riesgos Template.xlsx
</commit_message>
<xml_diff>
--- a/Matriz de Riesgos Template.xlsx
+++ b/Matriz de Riesgos Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2633D0-542D-44D1-93FB-122C391FCDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3877BC9B-B398-49E5-B12C-148C2361F6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1324,669 +1324,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Segoe UI Light"/>
         <scheme val="none"/>
@@ -2756,6 +2093,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3535,6 +2916,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -4452,6 +3877,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5369,6 +4838,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6286,6 +5799,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7093,6 +6650,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7900,6 +7501,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8713,6 +8358,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -9520,6 +9209,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -10333,6 +10066,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -11140,6 +10917,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -11947,6 +11768,50 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -12322,6 +12187,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12337,6 +12222,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12352,6 +12256,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12367,6 +12290,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12382,6 +12325,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12397,6 +12359,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -12408,6 +12389,25 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -13897,62 +13897,62 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table23" displayName="Table23" ref="A2:G15" totalsRowCount="1" headerRowDxfId="416" dataDxfId="415" totalsRowDxfId="414">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Periodo" totalsRowLabel="Total" dataDxfId="413" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Exposición Top 5" dataDxfId="412" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Exposición Top 10" dataDxfId="411" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Exposición Total" totalsRowFunction="custom" dataDxfId="410" totalsRowDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Periodo" totalsRowLabel="Total" dataDxfId="413" totalsRowDxfId="412"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Exposición Top 5" dataDxfId="411" totalsRowDxfId="410"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Exposición Top 10" dataDxfId="409" totalsRowDxfId="408"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Exposición Total" totalsRowFunction="custom" dataDxfId="407" totalsRowDxfId="406">
       <totalsRowFormula>SUM(D3:D14)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Q Riesgos Gestionados" totalsRowFunction="custom" dataDxfId="409" totalsRowDxfId="2">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Q Riesgos Gestionados" totalsRowFunction="custom" dataDxfId="405" totalsRowDxfId="404">
       <totalsRowFormula>IF(COUNT(E4:E10)&lt;&gt;0,SUM(E4:E10),"")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Q Riesgos Ocurridos" totalsRowFunction="custom" dataDxfId="408" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Q Riesgos Ocurridos" totalsRowFunction="custom" dataDxfId="403" totalsRowDxfId="402">
       <totalsRowFormula>IF(COUNT(F4:F10)&lt;&gt;0,SUM(F4:F10),"")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Impacto Riesgos Ocurridos" dataDxfId="407" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Impacto Riesgos Ocurridos" dataDxfId="401" totalsRowDxfId="400"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tblMatrizRiesgo714" displayName="tblMatrizRiesgo714" ref="B6:W27" totalsRowShown="0" headerRowDxfId="331" headerRowBorderDxfId="330" tableBorderDxfId="329" totalsRowBorderDxfId="328">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tblMatrizRiesgo714" displayName="tblMatrizRiesgo714" ref="B6:W27" totalsRowShown="0" headerRowDxfId="309" headerRowBorderDxfId="308" tableBorderDxfId="307" totalsRowBorderDxfId="306">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="ID" dataDxfId="327"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="326"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Categoria" dataDxfId="325"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="Equipo" dataDxfId="324"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0900-000018000000}" name="Sprint_x000a_(*)" dataDxfId="323"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="322"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Motivo_x000a_(*)" dataDxfId="321"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="320"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Impacto_x000a_(*)" dataDxfId="319"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="318"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Exposición del Riesgo" dataDxfId="317">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="ID" dataDxfId="305"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="304"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Categoria" dataDxfId="303"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="Equipo" dataDxfId="302"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0900-000018000000}" name="Sprint_x000a_(*)" dataDxfId="301"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="300"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Motivo_x000a_(*)" dataDxfId="299"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="298"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Impacto_x000a_(*)" dataDxfId="297"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="296"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Exposición del Riesgo" dataDxfId="295">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo714[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo714[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo714[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo714[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Severidad del Riesgo" dataDxfId="316">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Severidad del Riesgo" dataDxfId="294">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo714[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo714[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo714[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo714[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Estado_x000a_(*)" dataDxfId="315"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Plan de Contingencia" dataDxfId="314"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="313"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0900-000015000000}" name="Responsable_x000a_(*)" dataDxfId="312"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0900-000013000000}" name="Se notifica al cliente" dataDxfId="311"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Fecha de notificación al cliente" dataDxfId="310"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="309"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0900-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="308"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="307"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Aging" dataDxfId="306">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Estado_x000a_(*)" dataDxfId="293"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Plan de Contingencia" dataDxfId="292"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="291"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0900-000015000000}" name="Responsable_x000a_(*)" dataDxfId="290"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0900-000013000000}" name="Se notifica al cliente" dataDxfId="289"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Fecha de notificación al cliente" dataDxfId="288"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="287"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0900-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="286"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="285"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Aging" dataDxfId="284">
       <calculatedColumnFormula>IF(tblMatrizRiesgo714[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo714[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -13963,43 +13963,43 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="tblMatrizRiesgo715" displayName="tblMatrizRiesgo715" ref="B6:W27" totalsRowShown="0" headerRowDxfId="305" headerRowBorderDxfId="304" tableBorderDxfId="303" totalsRowBorderDxfId="302">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="tblMatrizRiesgo715" displayName="tblMatrizRiesgo715" ref="B6:W27" totalsRowShown="0" headerRowDxfId="278" headerRowBorderDxfId="277" tableBorderDxfId="276" totalsRowBorderDxfId="275">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="ID" dataDxfId="301"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="300"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0A00-00000F000000}" name="Categoria" dataDxfId="299"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0A00-00000D000000}" name="Equipo" dataDxfId="298"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0A00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="297"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="296"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0A00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="295"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="294"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="293"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="292"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="Exposición del Riesgo" dataDxfId="291">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="ID" dataDxfId="274"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="273"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0A00-00000F000000}" name="Categoria" dataDxfId="272"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0A00-00000D000000}" name="Equipo" dataDxfId="271"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0A00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="270"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="269"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0A00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="268"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="267"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="266"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="265"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="Exposición del Riesgo" dataDxfId="264">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo715[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo715[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo715[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo715[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0A00-00000E000000}" name="Severidad del Riesgo" dataDxfId="290">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0A00-00000E000000}" name="Severidad del Riesgo" dataDxfId="263">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo715[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo715[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo715[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo715[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="289"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Plan de Contingencia" dataDxfId="288"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="287"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0A00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="286"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0A00-000013000000}" name="Se notifica al cliente" dataDxfId="285"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0A00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="284"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="283"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0A00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="282"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="281"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0A00-000010000000}" name="Aging" dataDxfId="280">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="262"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Plan de Contingencia" dataDxfId="261"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="260"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0A00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="259"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0A00-000013000000}" name="Se notifica al cliente" dataDxfId="258"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0A00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="257"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="256"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0A00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="255"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="254"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0A00-000010000000}" name="Aging" dataDxfId="253">
       <calculatedColumnFormula>IF(tblMatrizRiesgo715[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo715[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14010,43 +14010,43 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="tblMatrizRiesgo716" displayName="tblMatrizRiesgo716" ref="B6:W27" totalsRowShown="0" headerRowDxfId="279" headerRowBorderDxfId="278" tableBorderDxfId="277" totalsRowBorderDxfId="276">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="tblMatrizRiesgo716" displayName="tblMatrizRiesgo716" ref="B6:W27" totalsRowShown="0" headerRowDxfId="247" headerRowBorderDxfId="246" tableBorderDxfId="245" totalsRowBorderDxfId="244">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="ID" dataDxfId="275"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="274"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0B00-00000F000000}" name="Categoria" dataDxfId="273"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0B00-00000D000000}" name="Equipo" dataDxfId="272"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0B00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="271"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="270"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0B00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="269"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="268"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="267"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="266"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="Exposición del Riesgo" dataDxfId="265">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="ID" dataDxfId="243"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="242"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0B00-00000F000000}" name="Categoria" dataDxfId="241"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0B00-00000D000000}" name="Equipo" dataDxfId="240"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0B00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="239"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="238"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0B00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="237"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="236"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="235"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="234"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="Exposición del Riesgo" dataDxfId="233">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo716[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo716[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo716[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo716[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0B00-00000E000000}" name="Severidad del Riesgo" dataDxfId="264">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0B00-00000E000000}" name="Severidad del Riesgo" dataDxfId="232">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo716[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo716[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo716[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo716[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0B00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="263"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Plan de Contingencia" dataDxfId="262"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="261"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0B00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="260"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0B00-000013000000}" name="Se notifica al cliente" dataDxfId="259"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0B00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="258"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="257"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0B00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="256"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="255"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0B00-000010000000}" name="Aging" dataDxfId="254">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0B00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="231"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Plan de Contingencia" dataDxfId="230"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="229"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0B00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="228"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0B00-000013000000}" name="Se notifica al cliente" dataDxfId="227"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0B00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="226"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="225"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0B00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="224"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="223"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0B00-000010000000}" name="Aging" dataDxfId="222">
       <calculatedColumnFormula>IF(tblMatrizRiesgo716[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo716[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14057,43 +14057,43 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="tblMatrizRiesgo717" displayName="tblMatrizRiesgo717" ref="B6:W27" totalsRowShown="0" headerRowDxfId="253" headerRowBorderDxfId="252" tableBorderDxfId="251" totalsRowBorderDxfId="250">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="tblMatrizRiesgo717" displayName="tblMatrizRiesgo717" ref="B6:W27" totalsRowShown="0" headerRowDxfId="216" headerRowBorderDxfId="215" tableBorderDxfId="214" totalsRowBorderDxfId="213">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="ID" dataDxfId="249"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="248"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0C00-00000F000000}" name="Categoria" dataDxfId="247"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0C00-00000D000000}" name="Equipo" dataDxfId="246"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0C00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="245"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="244"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0C00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="243"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="242"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="241"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="240"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Exposición del Riesgo" dataDxfId="239">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="ID" dataDxfId="212"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="211"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0C00-00000F000000}" name="Categoria" dataDxfId="210"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0C00-00000D000000}" name="Equipo" dataDxfId="209"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0C00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="208"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="207"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0C00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="206"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="205"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="204"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="203"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Exposición del Riesgo" dataDxfId="202">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo717[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo717[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo717[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo717[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0C00-00000E000000}" name="Severidad del Riesgo" dataDxfId="238">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0C00-00000E000000}" name="Severidad del Riesgo" dataDxfId="201">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo717[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo717[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo717[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo717[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0C00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="237"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Plan de Contingencia" dataDxfId="236"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="235"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0C00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="234"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0C00-000013000000}" name="Se notifica al cliente" dataDxfId="233"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0C00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="232"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="231"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0C00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="230"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0C00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="229"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0C00-000010000000}" name="Aging" dataDxfId="228">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0C00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Plan de Contingencia" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="198"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0C00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="197"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0C00-000013000000}" name="Se notifica al cliente" dataDxfId="196"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0C00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="195"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="194"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0C00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="193"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0C00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="192"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0C00-000010000000}" name="Aging" dataDxfId="191">
       <calculatedColumnFormula>IF(tblMatrizRiesgo717[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo717[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14104,43 +14104,43 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="tblMatrizRiesgo718" displayName="tblMatrizRiesgo718" ref="B6:W27" totalsRowShown="0" headerRowDxfId="227" headerRowBorderDxfId="226" tableBorderDxfId="225" totalsRowBorderDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="tblMatrizRiesgo718" displayName="tblMatrizRiesgo718" ref="B6:W27" totalsRowShown="0" headerRowDxfId="185" headerRowBorderDxfId="184" tableBorderDxfId="183" totalsRowBorderDxfId="182">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="ID" dataDxfId="223"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="222"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0D00-00000F000000}" name="Categoria" dataDxfId="221"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0D00-00000D000000}" name="Equipo" dataDxfId="220"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0D00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="219"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="218"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0D00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="217"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="216"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="215"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="214"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Exposición del Riesgo" dataDxfId="213">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="ID" dataDxfId="181"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="180"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0D00-00000F000000}" name="Categoria" dataDxfId="179"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0D00-00000D000000}" name="Equipo" dataDxfId="178"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0D00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="177"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="176"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0D00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="175"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="174"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="173"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="172"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="Exposición del Riesgo" dataDxfId="171">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo718[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo718[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo718[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo718[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0D00-00000E000000}" name="Severidad del Riesgo" dataDxfId="212">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0D00-00000E000000}" name="Severidad del Riesgo" dataDxfId="170">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo718[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo718[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo718[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo718[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0D00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="211"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Plan de Contingencia" dataDxfId="210"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="209"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0D00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="208"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0D00-000013000000}" name="Se notifica al cliente" dataDxfId="207"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0D00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="206"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="205"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0D00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="204"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0D00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="203"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0D00-000010000000}" name="Aging" dataDxfId="202">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0D00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="169"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Plan de Contingencia" dataDxfId="168"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="167"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0D00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="166"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0D00-000013000000}" name="Se notifica al cliente" dataDxfId="165"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0D00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="164"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="163"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0D00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="162"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0D00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="161"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0D00-000010000000}" name="Aging" dataDxfId="160">
       <calculatedColumnFormula>IF(tblMatrizRiesgo718[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo718[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14151,43 +14151,43 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="tblMatrizRiesgo719" displayName="tblMatrizRiesgo719" ref="B6:W27" totalsRowShown="0" headerRowDxfId="201" dataDxfId="199" headerRowBorderDxfId="200" tableBorderDxfId="198" totalsRowBorderDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="tblMatrizRiesgo719" displayName="tblMatrizRiesgo719" ref="B6:W27" totalsRowShown="0" headerRowDxfId="154" dataDxfId="152" headerRowBorderDxfId="153" tableBorderDxfId="151" totalsRowBorderDxfId="150">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="ID" dataDxfId="196"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="195"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Categoria" dataDxfId="194"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="Equipo" dataDxfId="193"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0E00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="192"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="191"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="190"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="189"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="188"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="187"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="Exposición del Riesgo" dataDxfId="186">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="ID" dataDxfId="149"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="148"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Categoria" dataDxfId="147"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="Equipo" dataDxfId="146"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0E00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="144"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="142"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="140"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="Exposición del Riesgo" dataDxfId="139">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo719[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo719[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo719[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo719[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="Severidad del Riesgo" dataDxfId="185">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="Severidad del Riesgo" dataDxfId="138">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo719[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo719[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo719[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo719[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="184"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Plan de Contingencia" dataDxfId="183"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="182"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0E00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="181"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0E00-000013000000}" name="Se notifica al cliente" dataDxfId="180"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="179"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="178"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0E00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="177"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="176"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Aging" dataDxfId="175">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Plan de Contingencia" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="135"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0E00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="134"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0E00-000013000000}" name="Se notifica al cliente" dataDxfId="133"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="132"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="131"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0E00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="130"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="129"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Aging" dataDxfId="128">
       <calculatedColumnFormula>IF(tblMatrizRiesgo719[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo719[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14198,43 +14198,43 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="tblMatrizRiesgo7192" displayName="tblMatrizRiesgo7192" ref="B6:W27" totalsRowShown="0" headerRowDxfId="174" dataDxfId="172" headerRowBorderDxfId="173" tableBorderDxfId="171" totalsRowBorderDxfId="170">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="tblMatrizRiesgo7192" displayName="tblMatrizRiesgo7192" ref="B6:W27" totalsRowShown="0" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121" tableBorderDxfId="119" totalsRowBorderDxfId="118">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="ID" dataDxfId="169"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="168"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0F00-00000F000000}" name="Categoria" dataDxfId="167"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0F00-00000D000000}" name="Equipo" dataDxfId="166"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0F00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="164"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0F00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="163"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="162"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="161"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0F00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="160"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="Exposición del Riesgo" dataDxfId="159">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="ID" dataDxfId="117"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="116"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0F00-00000F000000}" name="Categoria" dataDxfId="115"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0F00-00000D000000}" name="Equipo" dataDxfId="114"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0F00-000018000000}" name="Sprint_x000a_(*)" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="112"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0F00-000011000000}" name="Motivo_x000a_(*)" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="Impacto_x000a_(*)" dataDxfId="109"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0F00-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="108"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="Exposición del Riesgo" dataDxfId="107">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0F00-00000E000000}" name="Severidad del Riesgo" dataDxfId="158">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0F00-00000E000000}" name="Severidad del Riesgo" dataDxfId="106">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7192[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0F00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="157"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Plan de Contingencia" dataDxfId="156"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="155"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0F00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="154"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0F00-000013000000}" name="Se notifica al cliente" dataDxfId="153"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0F00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="152"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0F00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="151"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0F00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="150"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0F00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="149"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0F00-000010000000}" name="Aging" dataDxfId="148">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0F00-00000C000000}" name="Estado_x000a_(*)" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Plan de Contingencia" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="103"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0F00-000015000000}" name="Responsable_x000a_(*)" dataDxfId="102"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0F00-000013000000}" name="Se notifica al cliente" dataDxfId="101"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0F00-000012000000}" name="Fecha de notificación al cliente" dataDxfId="100"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0F00-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="99"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0F00-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="98"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0F00-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="97"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0F00-000010000000}" name="Aging" dataDxfId="96">
       <calculatedColumnFormula>IF(tblMatrizRiesgo7192[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo7192[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14245,43 +14245,43 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tblMatrizRiesgo71929" displayName="tblMatrizRiesgo71929" ref="B6:W27" totalsRowShown="0" headerRowDxfId="147" dataDxfId="145" headerRowBorderDxfId="146" tableBorderDxfId="144" totalsRowBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tblMatrizRiesgo71929" displayName="tblMatrizRiesgo71929" ref="B6:W27" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87" totalsRowBorderDxfId="86">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="ID" dataDxfId="142"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="141"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1000-00000F000000}" name="Categoria" dataDxfId="140"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1000-00000D000000}" name="Equipo" dataDxfId="139"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1000-000018000000}" name="Sprint_x000a_(*)" dataDxfId="138"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="137"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1000-000011000000}" name="Motivo_x000a_(*)" dataDxfId="136"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="135"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Impacto_x000a_(*)" dataDxfId="134"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="133"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="Exposición del Riesgo" dataDxfId="132">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="ID" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="84"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1000-00000F000000}" name="Categoria" dataDxfId="83"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1000-00000D000000}" name="Equipo" dataDxfId="82"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1000-000018000000}" name="Sprint_x000a_(*)" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1000-000011000000}" name="Motivo_x000a_(*)" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Impacto_x000a_(*)" dataDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="76"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="Exposición del Riesgo" dataDxfId="75">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1000-00000E000000}" name="Severidad del Riesgo" dataDxfId="131">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1000-00000E000000}" name="Severidad del Riesgo" dataDxfId="74">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo71929[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1000-00000C000000}" name="Estado_x000a_(*)" dataDxfId="130"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Plan de Contingencia" dataDxfId="129"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="128"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1000-000015000000}" name="Responsable_x000a_(*)" dataDxfId="127"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1000-000013000000}" name="Se notifica al cliente" dataDxfId="126"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1000-000012000000}" name="Fecha de notificación al cliente" dataDxfId="125"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="124"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1000-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="123"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="122"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1000-000010000000}" name="Aging" dataDxfId="121">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1000-00000C000000}" name="Estado_x000a_(*)" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Plan de Contingencia" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="71"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1000-000015000000}" name="Responsable_x000a_(*)" dataDxfId="70"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1000-000013000000}" name="Se notifica al cliente" dataDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1000-000012000000}" name="Fecha de notificación al cliente" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="67"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1000-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="65"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1000-000010000000}" name="Aging" dataDxfId="64">
       <calculatedColumnFormula>IF(tblMatrizRiesgo71929[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo71929[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14292,43 +14292,43 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tblMatrizRiesgo7192911" displayName="tblMatrizRiesgo7192911" ref="B6:W27" totalsRowShown="0" headerRowDxfId="120" dataDxfId="118" headerRowBorderDxfId="119" tableBorderDxfId="117" totalsRowBorderDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tblMatrizRiesgo7192911" displayName="tblMatrizRiesgo7192911" ref="B6:W27" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="ID" dataDxfId="115"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Categoria" dataDxfId="113"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Equipo" dataDxfId="112"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1100-000018000000}" name="Sprint_x000a_(*)" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="110"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Motivo_x000a_(*)" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Impacto_x000a_(*)" dataDxfId="107"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="106"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Exposición del Riesgo" dataDxfId="105">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="ID" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Categoria" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Equipo" dataDxfId="50"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1100-000018000000}" name="Sprint_x000a_(*)" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="48"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Motivo_x000a_(*)" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Impacto_x000a_(*)" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Exposición del Riesgo" dataDxfId="43">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Severidad del Riesgo" dataDxfId="104">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Severidad del Riesgo" dataDxfId="42">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7192911[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Estado_x000a_(*)" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="Plan de Contingencia" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="101"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Responsable_x000a_(*)" dataDxfId="100"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="Se notifica al cliente" dataDxfId="99"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="Fecha de notificación al cliente" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="97"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="95"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="Aging" dataDxfId="94">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Estado_x000a_(*)" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="Plan de Contingencia" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="39"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Responsable_x000a_(*)" dataDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="Se notifica al cliente" dataDxfId="37"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="Fecha de notificación al cliente" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="35"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="Aging" dataDxfId="32">
       <calculatedColumnFormula>IF(tblMatrizRiesgo7192911[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo7192911[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14339,43 +14339,43 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="tblMatrizRiesgo719291113" displayName="tblMatrizRiesgo719291113" ref="B6:W27" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="tblMatrizRiesgo719291113" displayName="tblMatrizRiesgo719291113" ref="B6:W27" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="ID" dataDxfId="88"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="87"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1200-00000F000000}" name="Categoria" dataDxfId="86"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1200-00000D000000}" name="Equipo" dataDxfId="85"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1200-000018000000}" name="Sprint_x000a_(*)" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="83"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1200-000011000000}" name="Motivo_x000a_(*)" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="Impacto_x000a_(*)" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1200-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1200-000008000000}" name="Exposición del Riesgo" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="ID" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1200-00000F000000}" name="Categoria" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1200-00000D000000}" name="Equipo" dataDxfId="18"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-1200-000018000000}" name="Sprint_x000a_(*)" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1200-000011000000}" name="Motivo_x000a_(*)" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="Impacto_x000a_(*)" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1200-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1200-000008000000}" name="Exposición del Riesgo" dataDxfId="11">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1200-00000E000000}" name="Severidad del Riesgo" dataDxfId="77">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1200-00000E000000}" name="Severidad del Riesgo" dataDxfId="10">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo719291113[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1200-00000C000000}" name="Estado_x000a_(*)" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Plan de Contingencia" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="74"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1200-000015000000}" name="Responsable_x000a_(*)" dataDxfId="73"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1200-000013000000}" name="Se notifica al cliente" dataDxfId="72"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1200-000012000000}" name="Fecha de notificación al cliente" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1200-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="70"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1200-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1200-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="68"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1200-000010000000}" name="Aging" dataDxfId="67">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1200-00000C000000}" name="Estado_x000a_(*)" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Plan de Contingencia" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1200-000015000000}" name="Responsable_x000a_(*)" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1200-000013000000}" name="Se notifica al cliente" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1200-000012000000}" name="Fecha de notificación al cliente" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1200-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1200-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1200-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1200-000010000000}" name="Aging" dataDxfId="0">
       <calculatedColumnFormula>IF(tblMatrizRiesgo719291113[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo719291113[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14386,102 +14386,102 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblPonderaciónProbabilidad" displayName="tblPonderaciónProbabilidad" ref="B2:C7" totalsRowShown="0" headerRowDxfId="406" dataDxfId="405">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblPonderaciónProbabilidad" displayName="tblPonderaciónProbabilidad" ref="B2:C7" totalsRowShown="0" headerRowDxfId="399" dataDxfId="398">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Probabilidad" dataDxfId="404"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Ponderación" dataDxfId="403"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Probabilidad" dataDxfId="397"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Ponderación" dataDxfId="396"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblPonderaciónImpacto" displayName="tblPonderaciónImpacto" ref="B9:C14" totalsRowShown="0" headerRowDxfId="402" dataDxfId="401">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblPonderaciónImpacto" displayName="tblPonderaciónImpacto" ref="B9:C14" totalsRowShown="0" headerRowDxfId="395" dataDxfId="394">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Impacto" dataDxfId="400"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Ponderación" dataDxfId="399"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Impacto" dataDxfId="393"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Ponderación" dataDxfId="392"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblProximidad" displayName="tblProximidad" ref="M7:N10" totalsRowShown="0" headerRowDxfId="398" dataDxfId="397">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblProximidad" displayName="tblProximidad" ref="M7:N10" totalsRowShown="0" headerRowDxfId="391" dataDxfId="390">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Proximidad" dataDxfId="396"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Descripción" dataDxfId="395"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Proximidad" dataDxfId="389"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Descripción" dataDxfId="388"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblCategorizacionExpRiesgo" displayName="tblCategorizacionExpRiesgo" ref="M2:N5" totalsRowShown="0" headerRowDxfId="394" dataDxfId="393">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblCategorizacionExpRiesgo" displayName="tblCategorizacionExpRiesgo" ref="M2:N5" totalsRowShown="0" headerRowDxfId="387" dataDxfId="386">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Exposición" dataDxfId="392"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Categoria" dataDxfId="391"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Exposición" dataDxfId="385"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Categoria" dataDxfId="384"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tblCategorias" displayName="tblCategorias" ref="M12:M18" totalsRowShown="0" headerRowDxfId="390" dataDxfId="389">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tblCategorias" displayName="tblCategorias" ref="M12:M18" totalsRowShown="0" headerRowDxfId="383" dataDxfId="382">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Categoria" dataDxfId="388"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Categoria" dataDxfId="381"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table161" displayName="Table161" ref="P2:P16" totalsRowShown="0" headerRowDxfId="387" dataDxfId="385" headerRowBorderDxfId="386">
-  <autoFilter ref="P2:P16" xr:uid="{00000000-0009-0000-0100-00003C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table161" displayName="Table161" ref="P2:P20" totalsRowShown="0" headerRowDxfId="380" dataDxfId="378" headerRowBorderDxfId="379">
+  <autoFilter ref="P2:P20" xr:uid="{00000000-0009-0000-0100-00003C000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Feriados" dataDxfId="384"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Feriados" dataDxfId="377"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tblMatrizRiesgo7" displayName="tblMatrizRiesgo7" ref="B6:W27" totalsRowShown="0" headerRowDxfId="383" headerRowBorderDxfId="382" tableBorderDxfId="381" totalsRowBorderDxfId="380">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tblMatrizRiesgo7" displayName="tblMatrizRiesgo7" ref="B6:W27" totalsRowShown="0" headerRowDxfId="371" headerRowBorderDxfId="370" tableBorderDxfId="369" totalsRowBorderDxfId="368">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="ID_x000a_(*)" dataDxfId="379"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="378"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Categoria_x000a_(*)" dataDxfId="377"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Equipo" dataDxfId="376"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0700-000018000000}" name="Sprint" dataDxfId="375"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="374"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Motivo_x000a_(*)" dataDxfId="373"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="372"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Impacto_x000a_(*)" dataDxfId="371"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="370"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Exposición del Riesgo" dataDxfId="369">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="ID_x000a_(*)" dataDxfId="367"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="366"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Categoria_x000a_(*)" dataDxfId="365"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Equipo" dataDxfId="364"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0700-000018000000}" name="Sprint" dataDxfId="363"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="362"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Motivo_x000a_(*)" dataDxfId="361"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="360"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Impacto_x000a_(*)" dataDxfId="359"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="358"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Exposición del Riesgo" dataDxfId="357">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo7[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo7[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo7[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Severidad del Riesgo" dataDxfId="368">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Severidad del Riesgo" dataDxfId="356">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo7[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo7[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo7[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Estado_x000a_(*)" dataDxfId="367"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Plan de Contingencia _x000a_(*)" dataDxfId="366"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="365"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0700-000015000000}" name="Responsable_x000a_(*)" dataDxfId="364"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="Se notifica al cliente" dataDxfId="363"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Fecha de notificación al cliente" dataDxfId="362"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Comentarios" dataDxfId="361"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0700-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="360"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="359"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Aging" dataDxfId="358">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Estado_x000a_(*)" dataDxfId="355"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Plan de Contingencia _x000a_(*)" dataDxfId="354"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="353"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0700-000015000000}" name="Responsable_x000a_(*)" dataDxfId="352"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="Se notifica al cliente" dataDxfId="351"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Fecha de notificación al cliente" dataDxfId="350"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Comentarios" dataDxfId="349"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0700-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="348"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="347"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Aging" dataDxfId="346">
       <calculatedColumnFormula>IF(tblMatrizRiesgo7[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo7[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -14492,43 +14492,43 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tblMatrizRiesgo712" displayName="tblMatrizRiesgo712" ref="B6:W27" totalsRowShown="0" headerRowDxfId="357" headerRowBorderDxfId="356" tableBorderDxfId="355" totalsRowBorderDxfId="354">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tblMatrizRiesgo712" displayName="tblMatrizRiesgo712" ref="B6:W27" totalsRowShown="0" headerRowDxfId="340" headerRowBorderDxfId="339" tableBorderDxfId="338" totalsRowBorderDxfId="337">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:V27">
     <sortCondition ref="M7:M27"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="ID" dataDxfId="353"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="352"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Categoria" dataDxfId="351"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Equipo" dataDxfId="350"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0800-000018000000}" name="Sprint_x000a_(*)" dataDxfId="349"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="348"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Motivo_x000a_(*)" dataDxfId="347"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="346"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Impacto_x000a_(*)" dataDxfId="345"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="344"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Exposición del Riesgo" dataDxfId="343">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="ID" dataDxfId="336"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Alcance del Riesgo_x000a_(*)" dataDxfId="335"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Categoria" dataDxfId="334"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Equipo" dataDxfId="333"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0800-000018000000}" name="Sprint_x000a_(*)" dataDxfId="332"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Riesgo_x000a_(*)" dataDxfId="331"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Motivo_x000a_(*)" dataDxfId="330"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Prob. de Ocurrencia_x000a_(*)" dataDxfId="329"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Impacto_x000a_(*)" dataDxfId="328"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Proximidad_x000a_(*)" dataDxfId="327"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Exposición del Riesgo" dataDxfId="326">
       <calculatedColumnFormula>IF(ISERROR(ROUNDUP(VLOOKUP(tblMatrizRiesgo712[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo712[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)),0,(ROUNDUP(VLOOKUP(tblMatrizRiesgo712[[#This Row],[Prob. de Ocurrencia
 (*)]],tblPonderaciónProbabilidad[],2,FALSE)*VLOOKUP(tblMatrizRiesgo712[[#This Row],[Impacto
 (*)]],tblPonderaciónImpacto[],2,FALSE),2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Severidad del Riesgo" dataDxfId="342">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Severidad del Riesgo" dataDxfId="325">
       <calculatedColumnFormula>IF(ISERROR(+VLOOKUP(tblMatrizRiesgo712[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo712[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)),"",(+VLOOKUP(tblMatrizRiesgo712[[#This Row],[Proximidad
 (*)]],Configuración!$F$14:$I$16,MATCH(VLOOKUP(tblMatrizRiesgo712[[#This Row],[Exposición del Riesgo]],tblCategorizacionExpRiesgo[],2,TRUE),Configuración!$F$17:$I$17,0),FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Estado_x000a_(*)" dataDxfId="341"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Plan de Contingencia" dataDxfId="340"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="339"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0800-000015000000}" name="Responsable_x000a_(*)" dataDxfId="338"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="Se notifica al cliente" dataDxfId="337"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Fecha de notificación al cliente" dataDxfId="336"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="335"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0800-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="334"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="333"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Aging" dataDxfId="332">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Estado_x000a_(*)" dataDxfId="324"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Plan de Contingencia" dataDxfId="323"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Estrategia de Mitigación_x000a_(*)" dataDxfId="322"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0800-000015000000}" name="Responsable_x000a_(*)" dataDxfId="321"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="Se notifica al cliente" dataDxfId="320"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Fecha de notificación al cliente" dataDxfId="319"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Comentarios_x000a_(*)" dataDxfId="318"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0800-000014000000}" name="¿Ocurrió el riesgo?_x000a_(*)" dataDxfId="317"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Fecha Log_x000a_(*)" dataDxfId="316"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Aging" dataDxfId="315">
       <calculatedColumnFormula>IF(tblMatrizRiesgo712[[#This Row],[Fecha Log
 (*)]]&lt;&gt;"",NETWORKDAYS(tblMatrizRiesgo712[[#This Row],[Fecha Log
 (*)]],TODAY(),Table161[Feriados]),"")</calculatedColumnFormula>
@@ -16457,14 +16457,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="190" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="188" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16481,12 +16481,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17763,14 +17763,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="159" priority="6" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="7" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="157" priority="8" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17787,12 +17787,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19069,14 +19069,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="127" priority="6" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="7" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="125" priority="8" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19093,12 +19093,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20375,14 +20375,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="6" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="94" priority="7" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="8" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20399,12 +20399,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21681,14 +21681,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="6" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="7" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="8" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21705,12 +21705,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22987,14 +22987,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23011,12 +23011,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23497,9 +23497,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:P18"/>
+  <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -23553,7 +23555,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="24">
-        <v>42370</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23596,7 +23598,7 @@
         <v>21</v>
       </c>
       <c r="P4" s="24">
-        <v>42408</v>
+        <v>43885</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23637,7 +23639,7 @@
         <v>22</v>
       </c>
       <c r="P5" s="24">
-        <v>42409</v>
+        <v>43886</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23672,7 +23674,7 @@
         <v>0.4</v>
       </c>
       <c r="P6" s="24">
-        <v>42453</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23713,7 +23715,7 @@
         <v>35</v>
       </c>
       <c r="P7" s="24">
-        <v>42454</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -23748,7 +23750,7 @@
         <v>37</v>
       </c>
       <c r="P8" s="24">
-        <v>42462</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23780,7 +23782,7 @@
         <v>38</v>
       </c>
       <c r="P9" s="24">
-        <v>42491</v>
+        <v>43931</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23804,7 +23806,7 @@
         <v>36</v>
       </c>
       <c r="P10" s="24">
-        <v>42515</v>
+        <v>43952</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23815,7 +23817,7 @@
         <v>0.1</v>
       </c>
       <c r="P11" s="24">
-        <v>42541</v>
+        <v>43976</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23832,7 +23834,7 @@
         <v>16</v>
       </c>
       <c r="P12" s="24">
-        <v>42559</v>
+        <v>44002</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23846,7 +23848,7 @@
         <v>98</v>
       </c>
       <c r="P13" s="24">
-        <v>42560</v>
+        <v>44021</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23875,7 +23877,7 @@
         <v>99</v>
       </c>
       <c r="P14" s="24">
-        <v>42712</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -23896,7 +23898,7 @@
         <v>47</v>
       </c>
       <c r="P15" s="24">
-        <v>42713</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -23917,10 +23919,10 @@
         <v>17</v>
       </c>
       <c r="P16" s="24">
-        <v>42729</v>
-      </c>
-    </row>
-    <row r="17" spans="7:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="17" spans="7:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G17" s="18" t="s">
         <v>20</v>
       </c>
@@ -23933,8 +23935,11 @@
       <c r="M17" s="19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="7:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="24">
+        <v>44158</v>
+      </c>
+    </row>
+    <row r="18" spans="7:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G18" s="80" t="s">
         <v>41</v>
       </c>
@@ -23942,6 +23947,19 @@
       <c r="I18" s="80"/>
       <c r="M18" s="19" t="s">
         <v>101</v>
+      </c>
+      <c r="P18" s="24">
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="19" spans="7:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="24">
+        <v>44173</v>
+      </c>
+    </row>
+    <row r="20" spans="7:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="24">
+        <v>44190</v>
       </c>
     </row>
   </sheetData>
@@ -23970,7 +23988,7 @@
   <dimension ref="B2:XFB37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -25206,14 +25224,14 @@
     <mergeCell ref="B34:D34"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="376" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="375" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="374" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25230,12 +25248,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26512,14 +26530,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="61" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="345" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="344" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="343" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26536,12 +26554,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27818,14 +27836,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="314" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="313" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="312" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27842,12 +27860,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29124,14 +29142,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="51" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="283" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="281" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29148,12 +29166,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30430,14 +30448,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="252" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="250" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30454,12 +30472,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31736,14 +31754,14 @@
     <mergeCell ref="B35:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L27">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="221" priority="4" operator="greaterThanOrEqual">
       <formula>0.18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="5" operator="between">
       <formula>0.06</formula>
       <formula>0.17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="219" priority="6" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31760,12 +31778,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="2" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W27">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="1" operator="equal">
       <formula>30263</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>